<commit_message>
nuevo ajuste para las tablas de l bd
</commit_message>
<xml_diff>
--- a/data/registros/periodos/202512/20529929821/propuesta_202512.xlsx
+++ b/data/registros/periodos/202512/20529929821/propuesta_202512.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CB30"/>
+  <dimension ref="A1:CB19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1997,12 +1997,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1016727499001F0010000000153</t>
+          <t>2060920957801F0010000002267</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>01/11/2025</t>
+          <t>25/12/2025</t>
         </is>
       </c>
       <c r="F8" t="inlineStr"/>
@@ -2019,7 +2019,7 @@
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t>153</t>
+          <t>2267</t>
         </is>
       </c>
       <c r="K8" t="inlineStr"/>
@@ -2030,22 +2030,22 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>10167274990</t>
+          <t>20609209578</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>MONDRAGON PINTADO DEMECIO</t>
+          <t>LA COCINA CENTRAL SOCIEDAD ANONIMA CERRADA - LACOCE S.A.C.</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>11.82</t>
+          <t>90.90</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>1.18</t>
+          <t>9.10</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
@@ -2090,7 +2090,7 @@
       </c>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>13.00</t>
+          <t>100.00</t>
         </is>
       </c>
       <c r="Z8" t="inlineStr">
@@ -2187,12 +2187,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1016727499001F0010000000154</t>
+          <t>2060872299901F0020000011302</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>01/11/2025</t>
+          <t>20/12/2025</t>
         </is>
       </c>
       <c r="F9" t="inlineStr"/>
@@ -2203,13 +2203,13 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>F001</t>
+          <t>F002</t>
         </is>
       </c>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>11302</t>
         </is>
       </c>
       <c r="K9" t="inlineStr"/>
@@ -2220,22 +2220,22 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>10167274990</t>
+          <t>20608722999</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>MONDRAGON PINTADO DEMECIO</t>
+          <t>GIASAL SOCIEDAD ANONIMA CERRADA</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>11.82</t>
+          <t>73.64</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>1.18</t>
+          <t>7.36</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
@@ -2280,7 +2280,7 @@
       </c>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>13.00</t>
+          <t>81.00</t>
         </is>
       </c>
       <c r="Z9" t="inlineStr">
@@ -2377,19 +2377,15 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2052530784101F0010000000207</t>
+          <t>2060690136501F0040000006416</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>12/07/2025</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>12/07/2025</t>
-        </is>
-      </c>
+          <t>05/12/2025</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
           <t>01</t>
@@ -2397,13 +2393,13 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>F001</t>
+          <t>F004</t>
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr">
         <is>
-          <t>207</t>
+          <t>6416</t>
         </is>
       </c>
       <c r="K10" t="inlineStr"/>
@@ -2414,22 +2410,22 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>20525307841</t>
+          <t>20606901365</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>OPTICA VILEN&amp;#039;S E.I.R.L</t>
+          <t>REGENDA ITK CORPORACION S.R.L.</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>169.49</t>
+          <t>313.56</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>30.51</t>
+          <t>56.44</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
@@ -2474,7 +2470,7 @@
       </c>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>200.00</t>
+          <t>370.00</t>
         </is>
       </c>
       <c r="Z10" t="inlineStr">
@@ -2561,7 +2557,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ADOLFO JURADO CONTRATISTAS GENERALES E I R L</t>
+          <t>ADOLFO JURADO CONTRATISTAS GENERALES E.I.R.L.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -2571,12 +2567,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2060920957801F0010000002188</t>
+          <t>2060690136501F0040000006417</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>30/11/2025</t>
+          <t>05/12/2025</t>
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
@@ -2587,13 +2583,13 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>F001</t>
+          <t>F004</t>
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr">
         <is>
-          <t>2188</t>
+          <t>6417</t>
         </is>
       </c>
       <c r="K11" t="inlineStr"/>
@@ -2604,22 +2600,22 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>20609209578</t>
+          <t>20606901365</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>LA COCINA CENTRAL SOCIEDAD ANONIMA CERRADA - LACOCE S.A.C.</t>
+          <t>REGENDA ITK CORPORACION S.R.L.</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>45.45</t>
+          <t>296.61</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>4.55</t>
+          <t>53.39</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
@@ -2664,7 +2660,7 @@
       </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>50.00</t>
+          <t>350.00</t>
         </is>
       </c>
       <c r="Z11" t="inlineStr">
@@ -2751,7 +2747,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ADOLFO JURADO CONTRATISTAS GENERALES E I R L</t>
+          <t>ADOLFO JURADO CONTRATISTAS GENERALES E.I.R.L.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2761,12 +2757,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2060920957801F0010000002267</t>
+          <t>2039952009701F0050000012393</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>25/12/2025</t>
+          <t>09/12/2025</t>
         </is>
       </c>
       <c r="F12" t="inlineStr"/>
@@ -2777,13 +2773,13 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>F001</t>
+          <t>F005</t>
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr">
         <is>
-          <t>2267</t>
+          <t>12393</t>
         </is>
       </c>
       <c r="K12" t="inlineStr"/>
@@ -2794,22 +2790,22 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>20609209578</t>
+          <t>20399520097</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>LA COCINA CENTRAL SOCIEDAD ANONIMA CERRADA - LACOCE S.A.C.</t>
+          <t>REPRESENTACIONES MONTALVAN EIRL</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>90.90</t>
+          <t>195.34</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>9.10</t>
+          <t>35.16</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
@@ -2854,7 +2850,7 @@
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>230.50</t>
         </is>
       </c>
       <c r="Z12" t="inlineStr">
@@ -2941,7 +2937,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ADOLFO JURADO CONTRATISTAS GENERALES E I R L</t>
+          <t>ADOLFO JURADO CONTRATISTAS GENERALES E.I.R.L.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2951,15 +2947,19 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2060872299901F0020000011302</t>
+          <t>2012776527901F02O0000082088</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>20/12/2025</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
+          <t>15/12/2025</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>15/12/2025</t>
+        </is>
+      </c>
       <c r="G13" t="inlineStr">
         <is>
           <t>01</t>
@@ -2967,13 +2967,13 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>F002</t>
+          <t>F02O</t>
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
-          <t>11302</t>
+          <t>82088</t>
         </is>
       </c>
       <c r="K13" t="inlineStr"/>
@@ -2984,22 +2984,22 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>20608722999</t>
+          <t>20127765279</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>GIASAL SOCIEDAD ANONIMA CERRADA</t>
+          <t>COESTI S.A.</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>73.64</t>
+          <t>84.75</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>7.36</t>
+          <t>15.25</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
@@ -3044,7 +3044,7 @@
       </c>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>81.00</t>
+          <t>100.00</t>
         </is>
       </c>
       <c r="Z13" t="inlineStr">
@@ -3131,7 +3131,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ADOLFO JURADO CONTRATISTAS GENERALES E.I.R.L.</t>
+          <t>ADOLFO JURADO CONTRATISTAS GENERALES EIRL</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -3141,15 +3141,19 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2048388680301F0030000013169</t>
+          <t>2010004721801FI010017682247</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>12/07/2025</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr"/>
+          <t>06/12/2025</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>01/11/2025</t>
+        </is>
+      </c>
       <c r="G14" t="inlineStr">
         <is>
           <t>01</t>
@@ -3157,13 +3161,13 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>F003</t>
+          <t>FI01</t>
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr">
         <is>
-          <t>13169</t>
+          <t>17682247</t>
         </is>
       </c>
       <c r="K14" t="inlineStr"/>
@@ -3174,22 +3178,22 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>20483886803</t>
+          <t>20100047218</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>REGENDA H Y D INVERSIONES Y SERVICIOS E.I.R.L.</t>
+          <t>BANCO DE CREDITO DEL PERU</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>186.44</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>33.56</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
@@ -3214,7 +3218,7 @@
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>40.50</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
@@ -3234,7 +3238,7 @@
       </c>
       <c r="Y14" t="inlineStr">
         <is>
-          <t>220.00</t>
+          <t>40.50</t>
         </is>
       </c>
       <c r="Z14" t="inlineStr">
@@ -3321,7 +3325,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ADOLFO JURADO CONTRATISTAS GENERALES E.I.R.L.</t>
+          <t>ADOLFO JURADO CONTRATISTAS GENERALES EIRL</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -3331,15 +3335,19 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2048388680301F0030000013170</t>
+          <t>2060828033301FI640000508075</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>12/07/2025</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr"/>
+          <t>24/12/2025</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>24/12/2025</t>
+        </is>
+      </c>
       <c r="G15" t="inlineStr">
         <is>
           <t>01</t>
@@ -3347,13 +3355,13 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>F003</t>
+          <t>FI64</t>
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
-          <t>13170</t>
+          <t>508075</t>
         </is>
       </c>
       <c r="K15" t="inlineStr"/>
@@ -3364,22 +3372,22 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>20483886803</t>
+          <t>20608280333</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>REGENDA H Y D INVERSIONES Y SERVICIOS E.I.R.L.</t>
+          <t>COMPANIA HARD DISCOUNT S.A.C</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>161.02</t>
+          <t>16.10</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>28.98</t>
+          <t>2.90</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
@@ -3424,7 +3432,7 @@
       </c>
       <c r="Y15" t="inlineStr">
         <is>
-          <t>190.00</t>
+          <t>19.00</t>
         </is>
       </c>
       <c r="Z15" t="inlineStr">
@@ -3511,7 +3519,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ADOLFO JURADO CONTRATISTAS GENERALES E.I.R.L.</t>
+          <t>ADOLFO JURADO CONTRATISTAS GENERALES EIRL</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -3521,15 +3529,19 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1002626837601F0030000014748</t>
+          <t>2010004721801FN010040212960</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>05/11/2025</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr"/>
+          <t>16/12/2025</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>15/12/2025</t>
+        </is>
+      </c>
       <c r="G16" t="inlineStr">
         <is>
           <t>01</t>
@@ -3537,13 +3549,13 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>F003</t>
+          <t>FN01</t>
         </is>
       </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
-          <t>14748</t>
+          <t>40212960</t>
         </is>
       </c>
       <c r="K16" t="inlineStr"/>
@@ -3554,22 +3566,22 @@
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>10026268376</t>
+          <t>20100047218</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>EDWIN NAQUICHE LOPEZ</t>
+          <t>BANCO DE CREDITO DEL PERU</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>19.49</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>3.51</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
@@ -3594,7 +3606,7 @@
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>10.00</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
@@ -3614,7 +3626,7 @@
       </c>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>23.00</t>
+          <t>10.00</t>
         </is>
       </c>
       <c r="Z16" t="inlineStr">
@@ -3711,7 +3723,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2060690136501F0040000006416</t>
+          <t>2060690136507FN040000000239</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -3722,18 +3734,18 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>07</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>F004</t>
+          <t>FN04</t>
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr">
         <is>
-          <t>6416</t>
+          <t>239</t>
         </is>
       </c>
       <c r="K17" t="inlineStr"/>
@@ -3754,12 +3766,12 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>313.56</t>
+          <t>-313.56</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>56.44</t>
+          <t>-56.44</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
@@ -3804,7 +3816,7 @@
       </c>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>370.00</t>
+          <t>-370.00</t>
         </is>
       </c>
       <c r="Z17" t="inlineStr">
@@ -3817,11 +3829,27 @@
           <t>1.000</t>
         </is>
       </c>
-      <c r="AB17" t="inlineStr"/>
-      <c r="AC17" t="inlineStr"/>
-      <c r="AD17" t="inlineStr"/>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>05/12/2025</t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>F004</t>
+        </is>
+      </c>
       <c r="AE17" t="inlineStr"/>
-      <c r="AF17" t="inlineStr"/>
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>6416</t>
+        </is>
+      </c>
       <c r="AG17" t="inlineStr"/>
       <c r="AH17" t="inlineStr"/>
       <c r="AI17" t="inlineStr"/>
@@ -3832,7 +3860,11 @@
       </c>
       <c r="AK17" t="inlineStr"/>
       <c r="AL17" t="inlineStr"/>
-      <c r="AM17" t="inlineStr"/>
+      <c r="AM17" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
       <c r="AN17" t="inlineStr">
         <is>
           <t>1</t>
@@ -3901,7 +3933,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2060690136501F0040000006417</t>
+          <t>2060690136507FN040000000240</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -3912,18 +3944,18 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>07</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>F004</t>
+          <t>FN04</t>
         </is>
       </c>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
-          <t>6417</t>
+          <t>240</t>
         </is>
       </c>
       <c r="K18" t="inlineStr"/>
@@ -3944,12 +3976,12 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>296.61</t>
+          <t>-296.61</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>53.39</t>
+          <t>-53.39</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
@@ -3994,7 +4026,7 @@
       </c>
       <c r="Y18" t="inlineStr">
         <is>
-          <t>350.00</t>
+          <t>-350.00</t>
         </is>
       </c>
       <c r="Z18" t="inlineStr">
@@ -4007,11 +4039,27 @@
           <t>1.000</t>
         </is>
       </c>
-      <c r="AB18" t="inlineStr"/>
-      <c r="AC18" t="inlineStr"/>
-      <c r="AD18" t="inlineStr"/>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>05/12/2025</t>
+        </is>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="AD18" t="inlineStr">
+        <is>
+          <t>F004</t>
+        </is>
+      </c>
       <c r="AE18" t="inlineStr"/>
-      <c r="AF18" t="inlineStr"/>
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>6417</t>
+        </is>
+      </c>
       <c r="AG18" t="inlineStr"/>
       <c r="AH18" t="inlineStr"/>
       <c r="AI18" t="inlineStr"/>
@@ -4022,7 +4070,11 @@
       </c>
       <c r="AK18" t="inlineStr"/>
       <c r="AL18" t="inlineStr"/>
-      <c r="AM18" t="inlineStr"/>
+      <c r="AM18" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
       <c r="AN18" t="inlineStr">
         <is>
           <t>1</t>
@@ -4091,29 +4143,33 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2060690136501F0040000006418</t>
+          <t>2046753402614SB010586767525</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>05/12/2025</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr"/>
+          <t>01/12/2025</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>19/12/2025</t>
+        </is>
+      </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>14</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>F004</t>
+          <t>SB01</t>
         </is>
       </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
-          <t>6418</t>
+          <t>0586767525</t>
         </is>
       </c>
       <c r="K19" t="inlineStr"/>
@@ -4124,22 +4180,22 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>20606901365</t>
+          <t>20467534026</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>REGENDA ITK CORPORACION S.R.L.</t>
+          <t>America Móvil Perú S.A.C.</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>298.31</t>
+          <t>89.00</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>53.69</t>
+          <t>16.02</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
@@ -4184,7 +4240,7 @@
       </c>
       <c r="Y19" t="inlineStr">
         <is>
-          <t>352.00</t>
+          <t>105.02</t>
         </is>
       </c>
       <c r="Z19" t="inlineStr">
@@ -4192,17 +4248,17 @@
           <t>PEN</t>
         </is>
       </c>
-      <c r="AA19" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
+      <c r="AA19" t="inlineStr"/>
       <c r="AB19" t="inlineStr"/>
       <c r="AC19" t="inlineStr"/>
       <c r="AD19" t="inlineStr"/>
       <c r="AE19" t="inlineStr"/>
       <c r="AF19" t="inlineStr"/>
-      <c r="AG19" t="inlineStr"/>
+      <c r="AG19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="AH19" t="inlineStr"/>
       <c r="AI19" t="inlineStr"/>
       <c r="AJ19" t="inlineStr">
@@ -4263,2152 +4319,6 @@
       <c r="CA19" t="inlineStr"/>
       <c r="CB19" t="inlineStr"/>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>20529929821</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>ADOLFO JURADO CONTRATISTAS GENERALES E.I.R.L.</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>202512</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>2039952009701F0050000012393</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>09/12/2025</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>F005</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>12393</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>20399520097</t>
-        </is>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>REPRESENTACIONES MONTALVAN EIRL</t>
-        </is>
-      </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>195.34</t>
-        </is>
-      </c>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>35.16</t>
-        </is>
-      </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="T20" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="U20" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="V20" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="W20" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="X20" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="Y20" t="inlineStr">
-        <is>
-          <t>230.50</t>
-        </is>
-      </c>
-      <c r="Z20" t="inlineStr">
-        <is>
-          <t>PEN</t>
-        </is>
-      </c>
-      <c r="AA20" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="AB20" t="inlineStr"/>
-      <c r="AC20" t="inlineStr"/>
-      <c r="AD20" t="inlineStr"/>
-      <c r="AE20" t="inlineStr"/>
-      <c r="AF20" t="inlineStr"/>
-      <c r="AG20" t="inlineStr"/>
-      <c r="AH20" t="inlineStr"/>
-      <c r="AI20" t="inlineStr"/>
-      <c r="AJ20" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AK20" t="inlineStr"/>
-      <c r="AL20" t="inlineStr"/>
-      <c r="AM20" t="inlineStr"/>
-      <c r="AN20" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AO20" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AP20" t="inlineStr"/>
-      <c r="AQ20" t="inlineStr"/>
-      <c r="AR20" t="inlineStr"/>
-      <c r="AS20" t="inlineStr"/>
-      <c r="AT20" t="inlineStr"/>
-      <c r="AU20" t="inlineStr"/>
-      <c r="AV20" t="inlineStr"/>
-      <c r="AW20" t="inlineStr"/>
-      <c r="AX20" t="inlineStr"/>
-      <c r="AY20" t="inlineStr"/>
-      <c r="AZ20" t="inlineStr"/>
-      <c r="BA20" t="inlineStr"/>
-      <c r="BB20" t="inlineStr"/>
-      <c r="BC20" t="inlineStr"/>
-      <c r="BD20" t="inlineStr"/>
-      <c r="BE20" t="inlineStr"/>
-      <c r="BF20" t="inlineStr"/>
-      <c r="BG20" t="inlineStr"/>
-      <c r="BH20" t="inlineStr"/>
-      <c r="BI20" t="inlineStr"/>
-      <c r="BJ20" t="inlineStr"/>
-      <c r="BK20" t="inlineStr"/>
-      <c r="BL20" t="inlineStr"/>
-      <c r="BM20" t="inlineStr"/>
-      <c r="BN20" t="inlineStr"/>
-      <c r="BO20" t="inlineStr"/>
-      <c r="BP20" t="inlineStr"/>
-      <c r="BQ20" t="inlineStr"/>
-      <c r="BR20" t="inlineStr"/>
-      <c r="BS20" t="inlineStr"/>
-      <c r="BT20" t="inlineStr"/>
-      <c r="BU20" t="inlineStr"/>
-      <c r="BV20" t="inlineStr"/>
-      <c r="BW20" t="inlineStr"/>
-      <c r="BX20" t="inlineStr"/>
-      <c r="BY20" t="inlineStr"/>
-      <c r="BZ20" t="inlineStr"/>
-      <c r="CA20" t="inlineStr"/>
-      <c r="CB20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>20529929821</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>ADOLFO JURADO CONTRATISTAS GENERALES E I R L</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>202512</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>2060861598001F0060000000853</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>11/11/2025</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>F006</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>853</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>20608615980</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>NORTE ALIMENTOS INDUSTRIAS Y SERVICIOS SOCIEDAD ANONIMA CERRADA</t>
-        </is>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>17.27</t>
-        </is>
-      </c>
-      <c r="P21" t="inlineStr">
-        <is>
-          <t>1.73</t>
-        </is>
-      </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="R21" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="T21" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="U21" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="V21" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="W21" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="X21" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="Y21" t="inlineStr">
-        <is>
-          <t>19.00</t>
-        </is>
-      </c>
-      <c r="Z21" t="inlineStr">
-        <is>
-          <t>PEN</t>
-        </is>
-      </c>
-      <c r="AA21" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="AB21" t="inlineStr"/>
-      <c r="AC21" t="inlineStr"/>
-      <c r="AD21" t="inlineStr"/>
-      <c r="AE21" t="inlineStr"/>
-      <c r="AF21" t="inlineStr"/>
-      <c r="AG21" t="inlineStr"/>
-      <c r="AH21" t="inlineStr"/>
-      <c r="AI21" t="inlineStr"/>
-      <c r="AJ21" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AK21" t="inlineStr"/>
-      <c r="AL21" t="inlineStr"/>
-      <c r="AM21" t="inlineStr"/>
-      <c r="AN21" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AO21" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AP21" t="inlineStr"/>
-      <c r="AQ21" t="inlineStr"/>
-      <c r="AR21" t="inlineStr"/>
-      <c r="AS21" t="inlineStr"/>
-      <c r="AT21" t="inlineStr"/>
-      <c r="AU21" t="inlineStr"/>
-      <c r="AV21" t="inlineStr"/>
-      <c r="AW21" t="inlineStr"/>
-      <c r="AX21" t="inlineStr"/>
-      <c r="AY21" t="inlineStr"/>
-      <c r="AZ21" t="inlineStr"/>
-      <c r="BA21" t="inlineStr"/>
-      <c r="BB21" t="inlineStr"/>
-      <c r="BC21" t="inlineStr"/>
-      <c r="BD21" t="inlineStr"/>
-      <c r="BE21" t="inlineStr"/>
-      <c r="BF21" t="inlineStr"/>
-      <c r="BG21" t="inlineStr"/>
-      <c r="BH21" t="inlineStr"/>
-      <c r="BI21" t="inlineStr"/>
-      <c r="BJ21" t="inlineStr"/>
-      <c r="BK21" t="inlineStr"/>
-      <c r="BL21" t="inlineStr"/>
-      <c r="BM21" t="inlineStr"/>
-      <c r="BN21" t="inlineStr"/>
-      <c r="BO21" t="inlineStr"/>
-      <c r="BP21" t="inlineStr"/>
-      <c r="BQ21" t="inlineStr"/>
-      <c r="BR21" t="inlineStr"/>
-      <c r="BS21" t="inlineStr"/>
-      <c r="BT21" t="inlineStr"/>
-      <c r="BU21" t="inlineStr"/>
-      <c r="BV21" t="inlineStr"/>
-      <c r="BW21" t="inlineStr"/>
-      <c r="BX21" t="inlineStr"/>
-      <c r="BY21" t="inlineStr"/>
-      <c r="BZ21" t="inlineStr"/>
-      <c r="CA21" t="inlineStr"/>
-      <c r="CB21" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>20529929821</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>ADOLFO JURADO CONTRATISTAS GENERALES E.I.R.L.</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>202512</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>2012776527901F02O0000082088</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>15/12/2025</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>15/12/2025</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>F02O</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>82088</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>20127765279</t>
-        </is>
-      </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>COESTI S.A.</t>
-        </is>
-      </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>84.75</t>
-        </is>
-      </c>
-      <c r="P22" t="inlineStr">
-        <is>
-          <t>15.25</t>
-        </is>
-      </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="T22" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="U22" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="V22" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="W22" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="X22" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="Y22" t="inlineStr">
-        <is>
-          <t>100.00</t>
-        </is>
-      </c>
-      <c r="Z22" t="inlineStr">
-        <is>
-          <t>PEN</t>
-        </is>
-      </c>
-      <c r="AA22" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="AB22" t="inlineStr"/>
-      <c r="AC22" t="inlineStr"/>
-      <c r="AD22" t="inlineStr"/>
-      <c r="AE22" t="inlineStr"/>
-      <c r="AF22" t="inlineStr"/>
-      <c r="AG22" t="inlineStr"/>
-      <c r="AH22" t="inlineStr"/>
-      <c r="AI22" t="inlineStr"/>
-      <c r="AJ22" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AK22" t="inlineStr"/>
-      <c r="AL22" t="inlineStr"/>
-      <c r="AM22" t="inlineStr"/>
-      <c r="AN22" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AO22" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AP22" t="inlineStr"/>
-      <c r="AQ22" t="inlineStr"/>
-      <c r="AR22" t="inlineStr"/>
-      <c r="AS22" t="inlineStr"/>
-      <c r="AT22" t="inlineStr"/>
-      <c r="AU22" t="inlineStr"/>
-      <c r="AV22" t="inlineStr"/>
-      <c r="AW22" t="inlineStr"/>
-      <c r="AX22" t="inlineStr"/>
-      <c r="AY22" t="inlineStr"/>
-      <c r="AZ22" t="inlineStr"/>
-      <c r="BA22" t="inlineStr"/>
-      <c r="BB22" t="inlineStr"/>
-      <c r="BC22" t="inlineStr"/>
-      <c r="BD22" t="inlineStr"/>
-      <c r="BE22" t="inlineStr"/>
-      <c r="BF22" t="inlineStr"/>
-      <c r="BG22" t="inlineStr"/>
-      <c r="BH22" t="inlineStr"/>
-      <c r="BI22" t="inlineStr"/>
-      <c r="BJ22" t="inlineStr"/>
-      <c r="BK22" t="inlineStr"/>
-      <c r="BL22" t="inlineStr"/>
-      <c r="BM22" t="inlineStr"/>
-      <c r="BN22" t="inlineStr"/>
-      <c r="BO22" t="inlineStr"/>
-      <c r="BP22" t="inlineStr"/>
-      <c r="BQ22" t="inlineStr"/>
-      <c r="BR22" t="inlineStr"/>
-      <c r="BS22" t="inlineStr"/>
-      <c r="BT22" t="inlineStr"/>
-      <c r="BU22" t="inlineStr"/>
-      <c r="BV22" t="inlineStr"/>
-      <c r="BW22" t="inlineStr"/>
-      <c r="BX22" t="inlineStr"/>
-      <c r="BY22" t="inlineStr"/>
-      <c r="BZ22" t="inlineStr"/>
-      <c r="CA22" t="inlineStr"/>
-      <c r="CB22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>20529929821</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>ADOLFO JURADO CONTRATISTAS GENERALES E.I.R.L.</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>202512</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>2044109760401F2170000124386</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>13/07/2025</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>F217</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>124386</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>20441097604</t>
-        </is>
-      </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>MOTO REPUESTOS &amp;amp; AB SAC</t>
-        </is>
-      </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>33.05</t>
-        </is>
-      </c>
-      <c r="P23" t="inlineStr">
-        <is>
-          <t>5.95</t>
-        </is>
-      </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="R23" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="T23" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="U23" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="V23" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="W23" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="X23" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="Y23" t="inlineStr">
-        <is>
-          <t>39.00</t>
-        </is>
-      </c>
-      <c r="Z23" t="inlineStr">
-        <is>
-          <t>PEN</t>
-        </is>
-      </c>
-      <c r="AA23" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="AB23" t="inlineStr"/>
-      <c r="AC23" t="inlineStr"/>
-      <c r="AD23" t="inlineStr"/>
-      <c r="AE23" t="inlineStr"/>
-      <c r="AF23" t="inlineStr"/>
-      <c r="AG23" t="inlineStr"/>
-      <c r="AH23" t="inlineStr"/>
-      <c r="AI23" t="inlineStr"/>
-      <c r="AJ23" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AK23" t="inlineStr"/>
-      <c r="AL23" t="inlineStr"/>
-      <c r="AM23" t="inlineStr"/>
-      <c r="AN23" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AO23" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AP23" t="inlineStr"/>
-      <c r="AQ23" t="inlineStr"/>
-      <c r="AR23" t="inlineStr"/>
-      <c r="AS23" t="inlineStr"/>
-      <c r="AT23" t="inlineStr"/>
-      <c r="AU23" t="inlineStr"/>
-      <c r="AV23" t="inlineStr"/>
-      <c r="AW23" t="inlineStr"/>
-      <c r="AX23" t="inlineStr"/>
-      <c r="AY23" t="inlineStr"/>
-      <c r="AZ23" t="inlineStr"/>
-      <c r="BA23" t="inlineStr"/>
-      <c r="BB23" t="inlineStr"/>
-      <c r="BC23" t="inlineStr"/>
-      <c r="BD23" t="inlineStr"/>
-      <c r="BE23" t="inlineStr"/>
-      <c r="BF23" t="inlineStr"/>
-      <c r="BG23" t="inlineStr"/>
-      <c r="BH23" t="inlineStr"/>
-      <c r="BI23" t="inlineStr"/>
-      <c r="BJ23" t="inlineStr"/>
-      <c r="BK23" t="inlineStr"/>
-      <c r="BL23" t="inlineStr"/>
-      <c r="BM23" t="inlineStr"/>
-      <c r="BN23" t="inlineStr"/>
-      <c r="BO23" t="inlineStr"/>
-      <c r="BP23" t="inlineStr"/>
-      <c r="BQ23" t="inlineStr"/>
-      <c r="BR23" t="inlineStr"/>
-      <c r="BS23" t="inlineStr"/>
-      <c r="BT23" t="inlineStr"/>
-      <c r="BU23" t="inlineStr"/>
-      <c r="BV23" t="inlineStr"/>
-      <c r="BW23" t="inlineStr"/>
-      <c r="BX23" t="inlineStr"/>
-      <c r="BY23" t="inlineStr"/>
-      <c r="BZ23" t="inlineStr"/>
-      <c r="CA23" t="inlineStr"/>
-      <c r="CB23" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>20529929821</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>ADOLFO JURADO CONTRATISTAS GENERALES E.I.R.L.</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>202512</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>2044109760401F2530000025992</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>13/07/2025</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>F253</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>25992</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>20441097604</t>
-        </is>
-      </c>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t>MOTO REPUESTOS &amp;amp; AB SAC</t>
-        </is>
-      </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>28.64</t>
-        </is>
-      </c>
-      <c r="P24" t="inlineStr">
-        <is>
-          <t>5.16</t>
-        </is>
-      </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="T24" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="V24" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="W24" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="X24" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="Y24" t="inlineStr">
-        <is>
-          <t>33.80</t>
-        </is>
-      </c>
-      <c r="Z24" t="inlineStr">
-        <is>
-          <t>PEN</t>
-        </is>
-      </c>
-      <c r="AA24" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="AB24" t="inlineStr"/>
-      <c r="AC24" t="inlineStr"/>
-      <c r="AD24" t="inlineStr"/>
-      <c r="AE24" t="inlineStr"/>
-      <c r="AF24" t="inlineStr"/>
-      <c r="AG24" t="inlineStr"/>
-      <c r="AH24" t="inlineStr"/>
-      <c r="AI24" t="inlineStr"/>
-      <c r="AJ24" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AK24" t="inlineStr"/>
-      <c r="AL24" t="inlineStr"/>
-      <c r="AM24" t="inlineStr"/>
-      <c r="AN24" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AO24" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AP24" t="inlineStr"/>
-      <c r="AQ24" t="inlineStr"/>
-      <c r="AR24" t="inlineStr"/>
-      <c r="AS24" t="inlineStr"/>
-      <c r="AT24" t="inlineStr"/>
-      <c r="AU24" t="inlineStr"/>
-      <c r="AV24" t="inlineStr"/>
-      <c r="AW24" t="inlineStr"/>
-      <c r="AX24" t="inlineStr"/>
-      <c r="AY24" t="inlineStr"/>
-      <c r="AZ24" t="inlineStr"/>
-      <c r="BA24" t="inlineStr"/>
-      <c r="BB24" t="inlineStr"/>
-      <c r="BC24" t="inlineStr"/>
-      <c r="BD24" t="inlineStr"/>
-      <c r="BE24" t="inlineStr"/>
-      <c r="BF24" t="inlineStr"/>
-      <c r="BG24" t="inlineStr"/>
-      <c r="BH24" t="inlineStr"/>
-      <c r="BI24" t="inlineStr"/>
-      <c r="BJ24" t="inlineStr"/>
-      <c r="BK24" t="inlineStr"/>
-      <c r="BL24" t="inlineStr"/>
-      <c r="BM24" t="inlineStr"/>
-      <c r="BN24" t="inlineStr"/>
-      <c r="BO24" t="inlineStr"/>
-      <c r="BP24" t="inlineStr"/>
-      <c r="BQ24" t="inlineStr"/>
-      <c r="BR24" t="inlineStr"/>
-      <c r="BS24" t="inlineStr"/>
-      <c r="BT24" t="inlineStr"/>
-      <c r="BU24" t="inlineStr"/>
-      <c r="BV24" t="inlineStr"/>
-      <c r="BW24" t="inlineStr"/>
-      <c r="BX24" t="inlineStr"/>
-      <c r="BY24" t="inlineStr"/>
-      <c r="BZ24" t="inlineStr"/>
-      <c r="CA24" t="inlineStr"/>
-      <c r="CB24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>20529929821</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>ADOLFO JURADO CONTRATISTAS GENERALES E.I.R.L.</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>202512</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>2044109760401F2560000002853</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>20/03/2025</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>F256</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>2853</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>20441097604</t>
-        </is>
-      </c>
-      <c r="N25" t="inlineStr">
-        <is>
-          <t>MOTO REPUESTOS &amp;amp; AB SAC</t>
-        </is>
-      </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>21.61</t>
-        </is>
-      </c>
-      <c r="P25" t="inlineStr">
-        <is>
-          <t>3.89</t>
-        </is>
-      </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="T25" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="U25" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="V25" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="W25" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="X25" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="Y25" t="inlineStr">
-        <is>
-          <t>25.50</t>
-        </is>
-      </c>
-      <c r="Z25" t="inlineStr">
-        <is>
-          <t>PEN</t>
-        </is>
-      </c>
-      <c r="AA25" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="AB25" t="inlineStr"/>
-      <c r="AC25" t="inlineStr"/>
-      <c r="AD25" t="inlineStr"/>
-      <c r="AE25" t="inlineStr"/>
-      <c r="AF25" t="inlineStr"/>
-      <c r="AG25" t="inlineStr"/>
-      <c r="AH25" t="inlineStr"/>
-      <c r="AI25" t="inlineStr"/>
-      <c r="AJ25" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AK25" t="inlineStr"/>
-      <c r="AL25" t="inlineStr"/>
-      <c r="AM25" t="inlineStr"/>
-      <c r="AN25" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AO25" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AP25" t="inlineStr"/>
-      <c r="AQ25" t="inlineStr"/>
-      <c r="AR25" t="inlineStr"/>
-      <c r="AS25" t="inlineStr"/>
-      <c r="AT25" t="inlineStr"/>
-      <c r="AU25" t="inlineStr"/>
-      <c r="AV25" t="inlineStr"/>
-      <c r="AW25" t="inlineStr"/>
-      <c r="AX25" t="inlineStr"/>
-      <c r="AY25" t="inlineStr"/>
-      <c r="AZ25" t="inlineStr"/>
-      <c r="BA25" t="inlineStr"/>
-      <c r="BB25" t="inlineStr"/>
-      <c r="BC25" t="inlineStr"/>
-      <c r="BD25" t="inlineStr"/>
-      <c r="BE25" t="inlineStr"/>
-      <c r="BF25" t="inlineStr"/>
-      <c r="BG25" t="inlineStr"/>
-      <c r="BH25" t="inlineStr"/>
-      <c r="BI25" t="inlineStr"/>
-      <c r="BJ25" t="inlineStr"/>
-      <c r="BK25" t="inlineStr"/>
-      <c r="BL25" t="inlineStr"/>
-      <c r="BM25" t="inlineStr"/>
-      <c r="BN25" t="inlineStr"/>
-      <c r="BO25" t="inlineStr"/>
-      <c r="BP25" t="inlineStr"/>
-      <c r="BQ25" t="inlineStr"/>
-      <c r="BR25" t="inlineStr"/>
-      <c r="BS25" t="inlineStr"/>
-      <c r="BT25" t="inlineStr"/>
-      <c r="BU25" t="inlineStr"/>
-      <c r="BV25" t="inlineStr"/>
-      <c r="BW25" t="inlineStr"/>
-      <c r="BX25" t="inlineStr"/>
-      <c r="BY25" t="inlineStr"/>
-      <c r="BZ25" t="inlineStr"/>
-      <c r="CA25" t="inlineStr"/>
-      <c r="CB25" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>20529929821</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>ADOLFO JURADO CONTRATISTAS GENERALES EIRL</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>202512</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>2010004721801FI010017682247</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>06/12/2025</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>01/11/2025</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>FI01</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>17682247</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>20100047218</t>
-        </is>
-      </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>BANCO DE CREDITO DEL PERU</t>
-        </is>
-      </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="P26" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="T26" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="U26" t="inlineStr">
-        <is>
-          <t>40.50</t>
-        </is>
-      </c>
-      <c r="V26" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="W26" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="X26" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="Y26" t="inlineStr">
-        <is>
-          <t>40.50</t>
-        </is>
-      </c>
-      <c r="Z26" t="inlineStr">
-        <is>
-          <t>PEN</t>
-        </is>
-      </c>
-      <c r="AA26" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="AB26" t="inlineStr"/>
-      <c r="AC26" t="inlineStr"/>
-      <c r="AD26" t="inlineStr"/>
-      <c r="AE26" t="inlineStr"/>
-      <c r="AF26" t="inlineStr"/>
-      <c r="AG26" t="inlineStr"/>
-      <c r="AH26" t="inlineStr"/>
-      <c r="AI26" t="inlineStr"/>
-      <c r="AJ26" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AK26" t="inlineStr"/>
-      <c r="AL26" t="inlineStr"/>
-      <c r="AM26" t="inlineStr"/>
-      <c r="AN26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AO26" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AP26" t="inlineStr"/>
-      <c r="AQ26" t="inlineStr"/>
-      <c r="AR26" t="inlineStr"/>
-      <c r="AS26" t="inlineStr"/>
-      <c r="AT26" t="inlineStr"/>
-      <c r="AU26" t="inlineStr"/>
-      <c r="AV26" t="inlineStr"/>
-      <c r="AW26" t="inlineStr"/>
-      <c r="AX26" t="inlineStr"/>
-      <c r="AY26" t="inlineStr"/>
-      <c r="AZ26" t="inlineStr"/>
-      <c r="BA26" t="inlineStr"/>
-      <c r="BB26" t="inlineStr"/>
-      <c r="BC26" t="inlineStr"/>
-      <c r="BD26" t="inlineStr"/>
-      <c r="BE26" t="inlineStr"/>
-      <c r="BF26" t="inlineStr"/>
-      <c r="BG26" t="inlineStr"/>
-      <c r="BH26" t="inlineStr"/>
-      <c r="BI26" t="inlineStr"/>
-      <c r="BJ26" t="inlineStr"/>
-      <c r="BK26" t="inlineStr"/>
-      <c r="BL26" t="inlineStr"/>
-      <c r="BM26" t="inlineStr"/>
-      <c r="BN26" t="inlineStr"/>
-      <c r="BO26" t="inlineStr"/>
-      <c r="BP26" t="inlineStr"/>
-      <c r="BQ26" t="inlineStr"/>
-      <c r="BR26" t="inlineStr"/>
-      <c r="BS26" t="inlineStr"/>
-      <c r="BT26" t="inlineStr"/>
-      <c r="BU26" t="inlineStr"/>
-      <c r="BV26" t="inlineStr"/>
-      <c r="BW26" t="inlineStr"/>
-      <c r="BX26" t="inlineStr"/>
-      <c r="BY26" t="inlineStr"/>
-      <c r="BZ26" t="inlineStr"/>
-      <c r="CA26" t="inlineStr"/>
-      <c r="CB26" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>20529929821</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>ADOLFO JURADO CONTRATISTAS GENERALES EIRL</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>202512</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>2060828033301FI640000508075</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>24/12/2025</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>24/12/2025</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>FI64</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>508075</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="M27" t="inlineStr">
-        <is>
-          <t>20608280333</t>
-        </is>
-      </c>
-      <c r="N27" t="inlineStr">
-        <is>
-          <t>COMPANIA HARD DISCOUNT S.A.C</t>
-        </is>
-      </c>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>16.10</t>
-        </is>
-      </c>
-      <c r="P27" t="inlineStr">
-        <is>
-          <t>2.90</t>
-        </is>
-      </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="R27" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="T27" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="U27" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="V27" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="W27" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="X27" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="Y27" t="inlineStr">
-        <is>
-          <t>19.00</t>
-        </is>
-      </c>
-      <c r="Z27" t="inlineStr">
-        <is>
-          <t>PEN</t>
-        </is>
-      </c>
-      <c r="AA27" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="AB27" t="inlineStr"/>
-      <c r="AC27" t="inlineStr"/>
-      <c r="AD27" t="inlineStr"/>
-      <c r="AE27" t="inlineStr"/>
-      <c r="AF27" t="inlineStr"/>
-      <c r="AG27" t="inlineStr"/>
-      <c r="AH27" t="inlineStr"/>
-      <c r="AI27" t="inlineStr"/>
-      <c r="AJ27" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AK27" t="inlineStr"/>
-      <c r="AL27" t="inlineStr"/>
-      <c r="AM27" t="inlineStr"/>
-      <c r="AN27" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AO27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AP27" t="inlineStr"/>
-      <c r="AQ27" t="inlineStr"/>
-      <c r="AR27" t="inlineStr"/>
-      <c r="AS27" t="inlineStr"/>
-      <c r="AT27" t="inlineStr"/>
-      <c r="AU27" t="inlineStr"/>
-      <c r="AV27" t="inlineStr"/>
-      <c r="AW27" t="inlineStr"/>
-      <c r="AX27" t="inlineStr"/>
-      <c r="AY27" t="inlineStr"/>
-      <c r="AZ27" t="inlineStr"/>
-      <c r="BA27" t="inlineStr"/>
-      <c r="BB27" t="inlineStr"/>
-      <c r="BC27" t="inlineStr"/>
-      <c r="BD27" t="inlineStr"/>
-      <c r="BE27" t="inlineStr"/>
-      <c r="BF27" t="inlineStr"/>
-      <c r="BG27" t="inlineStr"/>
-      <c r="BH27" t="inlineStr"/>
-      <c r="BI27" t="inlineStr"/>
-      <c r="BJ27" t="inlineStr"/>
-      <c r="BK27" t="inlineStr"/>
-      <c r="BL27" t="inlineStr"/>
-      <c r="BM27" t="inlineStr"/>
-      <c r="BN27" t="inlineStr"/>
-      <c r="BO27" t="inlineStr"/>
-      <c r="BP27" t="inlineStr"/>
-      <c r="BQ27" t="inlineStr"/>
-      <c r="BR27" t="inlineStr"/>
-      <c r="BS27" t="inlineStr"/>
-      <c r="BT27" t="inlineStr"/>
-      <c r="BU27" t="inlineStr"/>
-      <c r="BV27" t="inlineStr"/>
-      <c r="BW27" t="inlineStr"/>
-      <c r="BX27" t="inlineStr"/>
-      <c r="BY27" t="inlineStr"/>
-      <c r="BZ27" t="inlineStr"/>
-      <c r="CA27" t="inlineStr"/>
-      <c r="CB27" t="inlineStr"/>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>20529929821</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>ADOLFO JURADO CONTRATISTAS GENERALES EIRL</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>202512</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>2010004721801FN010040212960</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>16/12/2025</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>15/12/2025</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>FN01</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>40212960</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>20100047218</t>
-        </is>
-      </c>
-      <c r="N28" t="inlineStr">
-        <is>
-          <t>BANCO DE CREDITO DEL PERU</t>
-        </is>
-      </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="P28" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="T28" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="U28" t="inlineStr">
-        <is>
-          <t>10.00</t>
-        </is>
-      </c>
-      <c r="V28" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="W28" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="X28" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="Y28" t="inlineStr">
-        <is>
-          <t>10.00</t>
-        </is>
-      </c>
-      <c r="Z28" t="inlineStr">
-        <is>
-          <t>PEN</t>
-        </is>
-      </c>
-      <c r="AA28" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="AB28" t="inlineStr"/>
-      <c r="AC28" t="inlineStr"/>
-      <c r="AD28" t="inlineStr"/>
-      <c r="AE28" t="inlineStr"/>
-      <c r="AF28" t="inlineStr"/>
-      <c r="AG28" t="inlineStr"/>
-      <c r="AH28" t="inlineStr"/>
-      <c r="AI28" t="inlineStr"/>
-      <c r="AJ28" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AK28" t="inlineStr"/>
-      <c r="AL28" t="inlineStr"/>
-      <c r="AM28" t="inlineStr"/>
-      <c r="AN28" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AO28" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AP28" t="inlineStr"/>
-      <c r="AQ28" t="inlineStr"/>
-      <c r="AR28" t="inlineStr"/>
-      <c r="AS28" t="inlineStr"/>
-      <c r="AT28" t="inlineStr"/>
-      <c r="AU28" t="inlineStr"/>
-      <c r="AV28" t="inlineStr"/>
-      <c r="AW28" t="inlineStr"/>
-      <c r="AX28" t="inlineStr"/>
-      <c r="AY28" t="inlineStr"/>
-      <c r="AZ28" t="inlineStr"/>
-      <c r="BA28" t="inlineStr"/>
-      <c r="BB28" t="inlineStr"/>
-      <c r="BC28" t="inlineStr"/>
-      <c r="BD28" t="inlineStr"/>
-      <c r="BE28" t="inlineStr"/>
-      <c r="BF28" t="inlineStr"/>
-      <c r="BG28" t="inlineStr"/>
-      <c r="BH28" t="inlineStr"/>
-      <c r="BI28" t="inlineStr"/>
-      <c r="BJ28" t="inlineStr"/>
-      <c r="BK28" t="inlineStr"/>
-      <c r="BL28" t="inlineStr"/>
-      <c r="BM28" t="inlineStr"/>
-      <c r="BN28" t="inlineStr"/>
-      <c r="BO28" t="inlineStr"/>
-      <c r="BP28" t="inlineStr"/>
-      <c r="BQ28" t="inlineStr"/>
-      <c r="BR28" t="inlineStr"/>
-      <c r="BS28" t="inlineStr"/>
-      <c r="BT28" t="inlineStr"/>
-      <c r="BU28" t="inlineStr"/>
-      <c r="BV28" t="inlineStr"/>
-      <c r="BW28" t="inlineStr"/>
-      <c r="BX28" t="inlineStr"/>
-      <c r="BY28" t="inlineStr"/>
-      <c r="BZ28" t="inlineStr"/>
-      <c r="CA28" t="inlineStr"/>
-      <c r="CB28" t="inlineStr"/>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>20529929821</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>ADOLFO JURADO CONTRATISTAS GENERALES E.I.R.L.</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>202512</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>2060690136507FN040000000239</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>05/12/2025</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>FN04</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>239</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>20606901365</t>
-        </is>
-      </c>
-      <c r="N29" t="inlineStr">
-        <is>
-          <t>REGENDA ITK CORPORACION S.R.L.</t>
-        </is>
-      </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>-313.56</t>
-        </is>
-      </c>
-      <c r="P29" t="inlineStr">
-        <is>
-          <t>-56.44</t>
-        </is>
-      </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="R29" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="S29" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="T29" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="U29" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="V29" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="W29" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="X29" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="Y29" t="inlineStr">
-        <is>
-          <t>-370.00</t>
-        </is>
-      </c>
-      <c r="Z29" t="inlineStr">
-        <is>
-          <t>PEN</t>
-        </is>
-      </c>
-      <c r="AA29" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="AB29" t="inlineStr">
-        <is>
-          <t>05/12/2025</t>
-        </is>
-      </c>
-      <c r="AC29" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="AD29" t="inlineStr">
-        <is>
-          <t>F004</t>
-        </is>
-      </c>
-      <c r="AE29" t="inlineStr"/>
-      <c r="AF29" t="inlineStr">
-        <is>
-          <t>6416</t>
-        </is>
-      </c>
-      <c r="AG29" t="inlineStr"/>
-      <c r="AH29" t="inlineStr"/>
-      <c r="AI29" t="inlineStr"/>
-      <c r="AJ29" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AK29" t="inlineStr"/>
-      <c r="AL29" t="inlineStr"/>
-      <c r="AM29" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="AN29" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AO29" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AP29" t="inlineStr"/>
-      <c r="AQ29" t="inlineStr"/>
-      <c r="AR29" t="inlineStr"/>
-      <c r="AS29" t="inlineStr"/>
-      <c r="AT29" t="inlineStr"/>
-      <c r="AU29" t="inlineStr"/>
-      <c r="AV29" t="inlineStr"/>
-      <c r="AW29" t="inlineStr"/>
-      <c r="AX29" t="inlineStr"/>
-      <c r="AY29" t="inlineStr"/>
-      <c r="AZ29" t="inlineStr"/>
-      <c r="BA29" t="inlineStr"/>
-      <c r="BB29" t="inlineStr"/>
-      <c r="BC29" t="inlineStr"/>
-      <c r="BD29" t="inlineStr"/>
-      <c r="BE29" t="inlineStr"/>
-      <c r="BF29" t="inlineStr"/>
-      <c r="BG29" t="inlineStr"/>
-      <c r="BH29" t="inlineStr"/>
-      <c r="BI29" t="inlineStr"/>
-      <c r="BJ29" t="inlineStr"/>
-      <c r="BK29" t="inlineStr"/>
-      <c r="BL29" t="inlineStr"/>
-      <c r="BM29" t="inlineStr"/>
-      <c r="BN29" t="inlineStr"/>
-      <c r="BO29" t="inlineStr"/>
-      <c r="BP29" t="inlineStr"/>
-      <c r="BQ29" t="inlineStr"/>
-      <c r="BR29" t="inlineStr"/>
-      <c r="BS29" t="inlineStr"/>
-      <c r="BT29" t="inlineStr"/>
-      <c r="BU29" t="inlineStr"/>
-      <c r="BV29" t="inlineStr"/>
-      <c r="BW29" t="inlineStr"/>
-      <c r="BX29" t="inlineStr"/>
-      <c r="BY29" t="inlineStr"/>
-      <c r="BZ29" t="inlineStr"/>
-      <c r="CA29" t="inlineStr"/>
-      <c r="CB29" t="inlineStr"/>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>20529929821</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>ADOLFO JURADO CONTRATISTAS GENERALES E.I.R.L.</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>202512</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>2060690136507FN040000000240</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>05/12/2025</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>FN04</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>20606901365</t>
-        </is>
-      </c>
-      <c r="N30" t="inlineStr">
-        <is>
-          <t>REGENDA ITK CORPORACION S.R.L.</t>
-        </is>
-      </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>-296.61</t>
-        </is>
-      </c>
-      <c r="P30" t="inlineStr">
-        <is>
-          <t>-53.39</t>
-        </is>
-      </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="R30" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="T30" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="U30" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="V30" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="W30" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="X30" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="Y30" t="inlineStr">
-        <is>
-          <t>-350.00</t>
-        </is>
-      </c>
-      <c r="Z30" t="inlineStr">
-        <is>
-          <t>PEN</t>
-        </is>
-      </c>
-      <c r="AA30" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="AB30" t="inlineStr">
-        <is>
-          <t>05/12/2025</t>
-        </is>
-      </c>
-      <c r="AC30" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="AD30" t="inlineStr">
-        <is>
-          <t>F004</t>
-        </is>
-      </c>
-      <c r="AE30" t="inlineStr"/>
-      <c r="AF30" t="inlineStr">
-        <is>
-          <t>6417</t>
-        </is>
-      </c>
-      <c r="AG30" t="inlineStr"/>
-      <c r="AH30" t="inlineStr"/>
-      <c r="AI30" t="inlineStr"/>
-      <c r="AJ30" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AK30" t="inlineStr"/>
-      <c r="AL30" t="inlineStr"/>
-      <c r="AM30" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="AN30" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AO30" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AP30" t="inlineStr"/>
-      <c r="AQ30" t="inlineStr"/>
-      <c r="AR30" t="inlineStr"/>
-      <c r="AS30" t="inlineStr"/>
-      <c r="AT30" t="inlineStr"/>
-      <c r="AU30" t="inlineStr"/>
-      <c r="AV30" t="inlineStr"/>
-      <c r="AW30" t="inlineStr"/>
-      <c r="AX30" t="inlineStr"/>
-      <c r="AY30" t="inlineStr"/>
-      <c r="AZ30" t="inlineStr"/>
-      <c r="BA30" t="inlineStr"/>
-      <c r="BB30" t="inlineStr"/>
-      <c r="BC30" t="inlineStr"/>
-      <c r="BD30" t="inlineStr"/>
-      <c r="BE30" t="inlineStr"/>
-      <c r="BF30" t="inlineStr"/>
-      <c r="BG30" t="inlineStr"/>
-      <c r="BH30" t="inlineStr"/>
-      <c r="BI30" t="inlineStr"/>
-      <c r="BJ30" t="inlineStr"/>
-      <c r="BK30" t="inlineStr"/>
-      <c r="BL30" t="inlineStr"/>
-      <c r="BM30" t="inlineStr"/>
-      <c r="BN30" t="inlineStr"/>
-      <c r="BO30" t="inlineStr"/>
-      <c r="BP30" t="inlineStr"/>
-      <c r="BQ30" t="inlineStr"/>
-      <c r="BR30" t="inlineStr"/>
-      <c r="BS30" t="inlineStr"/>
-      <c r="BT30" t="inlineStr"/>
-      <c r="BU30" t="inlineStr"/>
-      <c r="BV30" t="inlineStr"/>
-      <c r="BW30" t="inlineStr"/>
-      <c r="BX30" t="inlineStr"/>
-      <c r="BY30" t="inlineStr"/>
-      <c r="BZ30" t="inlineStr"/>
-      <c r="CA30" t="inlineStr"/>
-      <c r="CB30" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>